<commit_message>
Alterado texto informarmativo de limite no Excel Power Query
</commit_message>
<xml_diff>
--- a/tools/excel/cnpja-excel-power-query.xlsx
+++ b/tools/excel/cnpja-excel-power-query.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\MEGA\Projects\personal\api-cnpja-examples\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\MEGA\Projects\personal\api-cnpja-examples\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EE7AB8-00DC-46D8-B6FE-A2F6D227C2F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1D8A0F-5B93-453B-96C8-BF3040314F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="675" windowWidth="27360" windowHeight="19965" xr2:uid="{87A05204-6064-4856-A1E6-3E21511CE204}"/>
+    <workbookView xWindow="3660" yWindow="300" windowWidth="26535" windowHeight="20205" xr2:uid="{87A05204-6064-4856-A1E6-3E21511CE204}"/>
   </bookViews>
   <sheets>
     <sheet name="CNPJá!" sheetId="3" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>CNPJ</t>
   </si>
@@ -187,12 +187,6 @@
     <t>Linhas em Branco?</t>
   </si>
   <si>
-    <t>• 500 consultas por dia</t>
-  </si>
-  <si>
-    <t>• 10 consultas por minuto</t>
-  </si>
-  <si>
     <t>© CNPJá! 2020 • Todos os Direitos Reservados</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
   </si>
   <si>
     <t>_CNPJ</t>
-  </si>
-  <si>
-    <t>Caso ultrapasse uma destas restrições algumas linhas ficarão em branco:</t>
   </si>
   <si>
     <r>
@@ -401,9 +392,6 @@
     </r>
   </si>
   <si>
-    <t>Atual: v1.0.1</t>
-  </si>
-  <si>
     <t>Atividade Econômica Classificação</t>
   </si>
   <si>
@@ -414,6 +402,15 @@
   </si>
   <si>
     <t>xxxxxxxx-xxxx-xxxx-xxxx-xxxxxxxxxxxx-xxxxxxxx-xxxx-xxxx-xxxx-xxxxxxxxxxxx</t>
+  </si>
+  <si>
+    <t>O plano gratuito está restringido a 30 consultas por hora.</t>
+  </si>
+  <si>
+    <t>Caso ultrapasse esta restrição algumas linhas ficarão em branco.</t>
+  </si>
+  <si>
+    <t>Atual: v1.0.2</t>
   </si>
 </sst>
 </file>
@@ -2905,13 +2902,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2970,13 +2967,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3035,13 +3032,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3778,7 +3775,7 @@
   <dimension ref="B2:G1011"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:E15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3809,7 +3806,7 @@
     </row>
     <row r="8" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
@@ -3820,7 +3817,7 @@
     </row>
     <row r="9" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3832,7 +3829,7 @@
     </row>
     <row r="10" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -3873,7 +3870,7 @@
     </row>
     <row r="15" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -3885,7 +3882,7 @@
     </row>
     <row r="17" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G17" s="15"/>
     </row>
@@ -3897,52 +3894,52 @@
     </row>
     <row r="19" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G19" s="15"/>
     </row>
     <row r="20" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
-        <v>57</v>
+      <c r="G24" s="15"/>
+    </row>
+    <row r="25" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
+        <v>51</v>
       </c>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+      <c r="G25" s="15"/>
+    </row>
+    <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="15"/>
-    </row>
-    <row r="25" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="25" t="s">
-        <v>56</v>
-      </c>
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G27" s="15"/>
     </row>
@@ -3961,7 +3958,7 @@
     </row>
     <row r="30" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="25"/>
@@ -3970,7 +3967,7 @@
     </row>
     <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
@@ -3979,7 +3976,7 @@
     </row>
     <row r="32" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
@@ -3987,63 +3984,57 @@
       <c r="G32" s="15"/>
     </row>
     <row r="33" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="25" t="s">
-        <v>58</v>
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="31" t="s">
+        <v>28</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="23"/>
+      <c r="D34" s="31" t="s">
+        <v>31</v>
+      </c>
       <c r="G34" s="15"/>
     </row>
     <row r="35" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
-        <v>30</v>
+      <c r="B35" s="33" t="s">
+        <v>29</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="31" t="s">
-        <v>33</v>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="G35" s="15"/>
     </row>
     <row r="36" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="33" t="s">
-        <v>31</v>
+      <c r="B36" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G36" s="15"/>
     </row>
     <row r="37" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="25" t="s">
-        <v>32</v>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="G37" s="15"/>
+    </row>
+    <row r="38" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="15"/>
+    </row>
+    <row r="39" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="37" t="s">
+        <v>26</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="G38" s="15"/>
-    </row>
-    <row r="39" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
       <c r="G39" s="15"/>
     </row>
     <row r="40" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
       <c r="G40" s="15"/>
     </row>
     <row r="41" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6962,11 +6953,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
-    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="B15:E15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B36" r:id="rId1" xr:uid="{764E0002-E7C3-41F0-B42B-D7E9AF39DCA8}"/>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{764E0002-E7C3-41F0-B42B-D7E9AF39DCA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7038,7 +7029,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>3</v>
@@ -7047,13 +7038,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>5</v>
@@ -7095,37 +7086,37 @@
         <v>18</v>
       </c>
       <c r="W1" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="X1" s="20" t="s">
         <v>19</v>
       </c>
       <c r="Y1" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Z1" s="20" t="s">
         <v>10</v>
       </c>
       <c r="AA1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="17" t="s">
+      <c r="AD1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="17" t="s">
+      <c r="AE1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AF1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF1" s="17" t="s">
-        <v>44</v>
-      </c>
       <c r="AG1" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AH1" s="20" t="s">
         <v>20</v>
@@ -7240,13 +7231,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>5</v>
@@ -7288,22 +7279,22 @@
         <v>18</v>
       </c>
       <c r="V1" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="Z1" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA1" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB1" s="4" t="s">
         <v>20</v>
@@ -11658,16 +11649,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -11789,16 +11780,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>44</v>
-      </c>
       <c r="G1" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:60" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionado instruções verificação de e-mail no Power Query
</commit_message>
<xml_diff>
--- a/tools/excel/cnpja-excel-power-query.xlsx
+++ b/tools/excel/cnpja-excel-power-query.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etrod\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\MEGA\Projects\personal\api-cnpja-examples\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59426B77-9B29-47C1-BE11-E050EE2FDACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABADA62-7601-4955-A0FE-5A96C32FD1F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="1140" windowWidth="19875" windowHeight="19320" firstSheet="1" activeTab="1" xr2:uid="{87A05204-6064-4856-A1E6-3E21511CE204}"/>
+    <workbookView xWindow="4365" yWindow="1140" windowWidth="27885" windowHeight="19320" firstSheet="1" activeTab="1" xr2:uid="{87A05204-6064-4856-A1E6-3E21511CE204}"/>
   </bookViews>
   <sheets>
     <sheet name="Conta" sheetId="16" state="veryHidden" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Simples" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="cnpjaApiKey">Setup!$C$30</definedName>
+    <definedName name="cnpjaApiKey">Setup!$C$32</definedName>
     <definedName name="DadosExternos_1" localSheetId="0" hidden="1">Conta!$A$1:$B$2</definedName>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">Base!$A$1:$AT$2</definedName>
     <definedName name="ExternalData_1" localSheetId="6" hidden="1">CNAEs!$A$1:$F$2</definedName>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
   <si>
     <t>CNPJ</t>
   </si>
@@ -330,47 +330,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">• Acesse a página </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFCADDE6"/>
-        <rFont val="Segoe UI Semibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>Minha Conta</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Segoe UI Semibold"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> de nosso site clicando </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFF7F158"/>
-        <rFont val="Segoe UI Semibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>aqui</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Segoe UI Semibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>Lembre-se de salvar o arquivo para não precisar realizar estes procedimentos novamente.</t>
   </si>
   <si>
@@ -497,9 +456,6 @@
       </rPr>
       <t xml:space="preserve"> para checar atualizações</t>
     </r>
-  </si>
-  <si>
-    <t>Atual: v1.2.0</t>
   </si>
   <si>
     <r>
@@ -705,6 +661,96 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> foram executados corretamente.</t>
+    </r>
+  </si>
+  <si>
+    <t>Atual: v1.2.1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Crie uma conta gratuita em nosso site clicando </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFF7F158"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>aqui</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, e em seguida no botão </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFCADDE6"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>Entrar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Você receberá uma mensagem de boas-vinda em seu e-mail, clique em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFCADDE6"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>Verificar E-mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Acesse a página </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFF7F158"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>Minha Conta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI Semibold"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> de nosso site.</t>
     </r>
   </si>
 </sst>
@@ -1207,18 +1253,6 @@
       <alignment horizontal="right" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1239,7 +1273,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -3274,13 +3320,13 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFF7F158"/>
+      <color rgb="FFCADDE6"/>
       <color rgb="FF20303C"/>
       <color rgb="FF273743"/>
-      <color rgb="FFCADDE6"/>
       <color rgb="FF2D3E4A"/>
       <color rgb="FFFF5B5B"/>
       <color rgb="FF0FE791"/>
-      <color rgb="FFF7F158"/>
       <color rgb="FF2EFAFA"/>
       <color rgb="FF445E70"/>
       <color rgb="FFFF7979"/>
@@ -3479,16 +3525,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3504,7 +3550,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5124450" y="19716750"/>
+          <a:off x="4705350" y="6600825"/>
           <a:ext cx="419100" cy="238126"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3546,13 +3592,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>134863</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>484263</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3603,13 +3649,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>135255</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>483870</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>155669</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3660,13 +3706,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>314329</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>200023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>25925</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>141059</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3728,13 +3774,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>571503</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>28573</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>283099</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>217259</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3796,13 +3842,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>209554</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>66673</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>635525</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>7709</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3831,6 +3877,71 @@
           <a:solidFill>
             <a:srgbClr val="20303C"/>
           </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 22">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ED3BD65-35AB-4B40-838E-CA3817E6723F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2200275" y="7067550"/>
+          <a:ext cx="1085850" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -5009,10 +5120,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -9386,10 +9497,10 @@
   <sheetPr codeName="Planilha1">
     <tabColor rgb="FF20303C"/>
   </sheetPr>
-  <dimension ref="B6:M72"/>
+  <dimension ref="B6:M74"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:K30"/>
+      <selection activeCell="C32" sqref="C32:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9404,20 +9515,20 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
     </row>
     <row r="7" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="46"/>
@@ -9434,69 +9545,69 @@
       <c r="M7" s="46"/>
     </row>
     <row r="8" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="78" t="s">
-        <v>80</v>
+      <c r="B8" s="75" t="s">
+        <v>79</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
     </row>
     <row r="9" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
     </row>
     <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
     </row>
     <row r="12" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
     </row>
     <row r="14" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9514,84 +9625,92 @@
     <row r="23" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="76" t="s">
-        <v>91</v>
+      <c r="B25" s="73" t="s">
+        <v>89</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="76"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
     </row>
     <row r="26" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="44" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="44"/>
+    </row>
+    <row r="32" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
+    </row>
+    <row r="33" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="71"/>
+    </row>
+    <row r="36" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="69" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
-    </row>
-    <row r="30" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="75" t="s">
-        <v>47</v>
+    <row r="38" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="69" t="s">
+        <v>91</v>
       </c>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-    </row>
-    <row r="31" spans="2:13" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="74" t="s">
+    </row>
+    <row r="39" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-    </row>
-    <row r="34" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="69" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="69" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="69" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="40" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9601,144 +9720,146 @@
     <row r="46" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:13" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:13" s="49" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="72" t="s">
-        <v>95</v>
+    <row r="49" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:13" s="49" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="79" t="s">
+        <v>93</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="72"/>
-      <c r="H64" s="72"/>
-      <c r="I64" s="72"/>
-      <c r="J64" s="72"/>
-      <c r="K64" s="72"/>
-      <c r="L64" s="72"/>
-      <c r="M64" s="72"/>
-    </row>
-    <row r="65" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="50"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="50"/>
-      <c r="K65" s="50"/>
-      <c r="L65" s="50"/>
-      <c r="M65" s="50"/>
-    </row>
-    <row r="66" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="73" t="s">
+      <c r="C66" s="79"/>
+      <c r="D66" s="79"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="79"/>
+      <c r="G66" s="79"/>
+      <c r="H66" s="79"/>
+      <c r="I66" s="79"/>
+      <c r="J66" s="79"/>
+      <c r="K66" s="79"/>
+      <c r="L66" s="79"/>
+      <c r="M66" s="79"/>
+    </row>
+    <row r="67" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="50"/>
+      <c r="I67" s="50"/>
+      <c r="J67" s="50"/>
+      <c r="K67" s="50"/>
+      <c r="L67" s="50"/>
+      <c r="M67" s="50"/>
+    </row>
+    <row r="68" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="76"/>
+      <c r="D68" s="76"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="76"/>
+      <c r="G68" s="76"/>
+      <c r="H68" s="76"/>
+      <c r="I68" s="76"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="76"/>
+      <c r="L68" s="76"/>
+      <c r="M68" s="76"/>
+    </row>
+    <row r="69" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="76"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="76"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="76"/>
+      <c r="L69" s="76"/>
+      <c r="M69" s="76"/>
+    </row>
+    <row r="70" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="50"/>
+      <c r="K70" s="50"/>
+      <c r="L70" s="50"/>
+      <c r="M70" s="50"/>
+    </row>
+    <row r="71" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="73"/>
-      <c r="D66" s="73"/>
-      <c r="E66" s="73"/>
-      <c r="F66" s="73"/>
-      <c r="G66" s="73"/>
-      <c r="H66" s="73"/>
-      <c r="I66" s="73"/>
-      <c r="J66" s="73"/>
-      <c r="K66" s="73"/>
-      <c r="L66" s="73"/>
-      <c r="M66" s="73"/>
-    </row>
-    <row r="67" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" s="73"/>
-      <c r="D67" s="73"/>
-      <c r="E67" s="73"/>
-      <c r="F67" s="73"/>
-      <c r="G67" s="73"/>
-      <c r="H67" s="73"/>
-      <c r="I67" s="73"/>
-      <c r="J67" s="73"/>
-      <c r="K67" s="73"/>
-      <c r="L67" s="73"/>
-      <c r="M67" s="73"/>
-    </row>
-    <row r="68" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="50"/>
-      <c r="E68" s="50"/>
-      <c r="F68" s="50"/>
-      <c r="G68" s="50"/>
-      <c r="H68" s="50"/>
-      <c r="I68" s="50"/>
-      <c r="J68" s="50"/>
-      <c r="K68" s="50"/>
-      <c r="L68" s="50"/>
-      <c r="M68" s="50"/>
-    </row>
-    <row r="69" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="C69" s="73"/>
-      <c r="D69" s="73"/>
-      <c r="E69" s="73"/>
-      <c r="F69" s="73"/>
-      <c r="G69" s="73"/>
-      <c r="H69" s="73"/>
-      <c r="I69" s="73"/>
-      <c r="J69" s="73"/>
-      <c r="K69" s="73"/>
-      <c r="L69" s="73"/>
-      <c r="M69" s="73"/>
-    </row>
-    <row r="72" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="71" t="s">
+      <c r="C71" s="76"/>
+      <c r="D71" s="76"/>
+      <c r="E71" s="76"/>
+      <c r="F71" s="76"/>
+      <c r="G71" s="76"/>
+      <c r="H71" s="76"/>
+      <c r="I71" s="76"/>
+      <c r="J71" s="76"/>
+      <c r="K71" s="76"/>
+      <c r="L71" s="76"/>
+      <c r="M71" s="76"/>
+    </row>
+    <row r="74" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="71"/>
-      <c r="D72" s="71"/>
-      <c r="E72" s="71"/>
-      <c r="F72" s="71"/>
-      <c r="G72" s="71"/>
-      <c r="H72" s="71"/>
-      <c r="I72" s="71"/>
-      <c r="J72" s="71"/>
-      <c r="K72" s="71"/>
-      <c r="L72" s="71"/>
-      <c r="M72" s="71"/>
+      <c r="C74" s="78"/>
+      <c r="D74" s="78"/>
+      <c r="E74" s="78"/>
+      <c r="F74" s="78"/>
+      <c r="G74" s="78"/>
+      <c r="H74" s="78"/>
+      <c r="I74" s="78"/>
+      <c r="J74" s="78"/>
+      <c r="K74" s="78"/>
+      <c r="L74" s="78"/>
+      <c r="M74" s="78"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="C30:K30"/>
+    <mergeCell ref="B74:M74"/>
+    <mergeCell ref="B66:M66"/>
+    <mergeCell ref="B68:M68"/>
+    <mergeCell ref="B71:M71"/>
+    <mergeCell ref="B69:M69"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="C32:K32"/>
     <mergeCell ref="B25:M25"/>
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="B8:M8"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:M10"/>
     <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B72:M72"/>
-    <mergeCell ref="B64:M64"/>
-    <mergeCell ref="B66:M66"/>
-    <mergeCell ref="B69:M69"/>
-    <mergeCell ref="B67:M67"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9826,7 +9947,7 @@
         <v>0 registros</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F7" s="58"/>
     </row>
@@ -9838,7 +9959,7 @@
       <c r="C8" s="52"/>
       <c r="D8" s="20"/>
       <c r="E8" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F8" s="58"/>
     </row>
@@ -9899,7 +10020,7 @@
       <c r="C15" s="51"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F15" s="58"/>
     </row>
@@ -9991,7 +10112,7 @@
     <row r="27" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="61"/>
       <c r="E27" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" s="19"/>
     </row>
@@ -10052,7 +10173,7 @@
     <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="61"/>
       <c r="E36" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F36" s="63" t="s">
         <v>25</v>
@@ -10061,7 +10182,7 @@
     <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="61"/>
       <c r="E37" s="19" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F37" s="19"/>
     </row>

</xml_diff>

<commit_message>
Adicionado Guia na Excel Power Query
</commit_message>
<xml_diff>
--- a/tools/excel/cnpja-excel-power-query.xlsx
+++ b/tools/excel/cnpja-excel-power-query.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\MEGA\Projects\personal\cnpja-public\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE119CD5-CADF-425D-BEE5-DEDA5FD9FFE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFCCE42-2CC0-4C09-A9B2-90A4B5710692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="735" windowWidth="24660" windowHeight="18930" tabRatio="795" firstSheet="4" activeTab="4" xr2:uid="{87A05204-6064-4856-A1E6-3E21511CE204}"/>
   </bookViews>
@@ -2093,13 +2093,21 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2109,12 +2117,20 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -2142,22 +2158,6 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -35202,18 +35202,18 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
       <c r="L6" s="84"/>
       <c r="M6" s="84"/>
     </row>
@@ -35260,18 +35260,18 @@
       <c r="K9" s="88"/>
     </row>
     <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
       <c r="L10" s="83"/>
       <c r="M10" s="83"/>
     </row>
@@ -35470,17 +35470,17 @@
       <c r="B71" s="51"/>
     </row>
     <row r="72" spans="2:13" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="87" t="s">
+      <c r="B72" s="90" t="s">
         <v>117</v>
       </c>
-      <c r="C72" s="87"/>
-      <c r="D72" s="87"/>
-      <c r="E72" s="87"/>
-      <c r="F72" s="87"/>
-      <c r="G72" s="87"/>
-      <c r="H72" s="87"/>
-      <c r="I72" s="87"/>
-      <c r="J72" s="87"/>
+      <c r="C72" s="90"/>
+      <c r="D72" s="90"/>
+      <c r="E72" s="90"/>
+      <c r="F72" s="90"/>
+      <c r="G72" s="90"/>
+      <c r="H72" s="90"/>
+      <c r="I72" s="90"/>
+      <c r="J72" s="90"/>
     </row>
     <row r="73" spans="2:13" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="2:13" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -35543,18 +35543,18 @@
     <row r="104" spans="2:13" s="34" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="105" spans="2:13" s="34" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="107" spans="2:13" s="35" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="91" t="s">
+      <c r="B107" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="C107" s="91"/>
-      <c r="D107" s="91"/>
-      <c r="E107" s="91"/>
-      <c r="F107" s="91"/>
-      <c r="G107" s="91"/>
-      <c r="H107" s="91"/>
-      <c r="I107" s="91"/>
-      <c r="J107" s="91"/>
-      <c r="K107" s="91"/>
+      <c r="C107" s="87"/>
+      <c r="D107" s="87"/>
+      <c r="E107" s="87"/>
+      <c r="F107" s="87"/>
+      <c r="G107" s="87"/>
+      <c r="H107" s="87"/>
+      <c r="I107" s="87"/>
+      <c r="J107" s="87"/>
+      <c r="K107" s="87"/>
       <c r="L107" s="81"/>
       <c r="M107" s="81"/>
     </row>
@@ -35601,33 +35601,33 @@
       <c r="K110" s="88"/>
     </row>
     <row r="113" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="92" t="s">
+      <c r="B113" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="C113" s="92"/>
-      <c r="D113" s="92"/>
-      <c r="E113" s="92"/>
-      <c r="F113" s="92"/>
-      <c r="G113" s="92"/>
-      <c r="H113" s="92"/>
-      <c r="I113" s="92"/>
-      <c r="J113" s="92"/>
-      <c r="K113" s="92"/>
+      <c r="C113" s="89"/>
+      <c r="D113" s="89"/>
+      <c r="E113" s="89"/>
+      <c r="F113" s="89"/>
+      <c r="G113" s="89"/>
+      <c r="H113" s="89"/>
+      <c r="I113" s="89"/>
+      <c r="J113" s="89"/>
+      <c r="K113" s="89"/>
       <c r="L113" s="82"/>
       <c r="M113" s="82"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="9">
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B6:K6"/>
     <mergeCell ref="B107:K107"/>
     <mergeCell ref="B109:K109"/>
     <mergeCell ref="B110:K110"/>
     <mergeCell ref="B113:K113"/>
     <mergeCell ref="B72:J72"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="B6:K6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -35642,9 +35642,7 @@
   </sheetPr>
   <dimension ref="B6:M82"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -35658,18 +35656,18 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:13" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
       <c r="L6" s="84"/>
       <c r="M6" s="84"/>
     </row>
@@ -36038,18 +36036,18 @@
     </row>
     <row r="75" spans="2:13" s="34" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="2:13" s="35" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="91" t="s">
+      <c r="B77" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="91"/>
-      <c r="F77" s="91"/>
-      <c r="G77" s="91"/>
-      <c r="H77" s="91"/>
-      <c r="I77" s="91"/>
-      <c r="J77" s="91"/>
-      <c r="K77" s="91"/>
+      <c r="C77" s="87"/>
+      <c r="D77" s="87"/>
+      <c r="E77" s="87"/>
+      <c r="F77" s="87"/>
+      <c r="G77" s="87"/>
+      <c r="H77" s="87"/>
+      <c r="I77" s="87"/>
+      <c r="J77" s="87"/>
+      <c r="K77" s="87"/>
       <c r="L77" s="81"/>
       <c r="M77" s="81"/>
     </row>
@@ -36082,18 +36080,18 @@
       <c r="K79" s="88"/>
     </row>
     <row r="82" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="92" t="s">
+      <c r="B82" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="C82" s="92"/>
-      <c r="D82" s="92"/>
-      <c r="E82" s="92"/>
-      <c r="F82" s="92"/>
-      <c r="G82" s="92"/>
-      <c r="H82" s="92"/>
-      <c r="I82" s="92"/>
-      <c r="J82" s="92"/>
-      <c r="K82" s="92"/>
+      <c r="C82" s="89"/>
+      <c r="D82" s="89"/>
+      <c r="E82" s="89"/>
+      <c r="F82" s="89"/>
+      <c r="G82" s="89"/>
+      <c r="H82" s="89"/>
+      <c r="I82" s="89"/>
+      <c r="J82" s="89"/>
+      <c r="K82" s="89"/>
       <c r="L82" s="82"/>
       <c r="M82" s="82"/>
     </row>
@@ -36148,14 +36146,14 @@
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
       <c r="F2" s="39"/>
-      <c r="N2" s="100" t="str">
+      <c r="N2" s="93" t="str">
         <f>IFERROR(VLOOKUP("email",CNPJá___Conta[],2,0),"")</f>
         <v/>
       </c>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
       <c r="S2" s="68"/>
     </row>
     <row r="3" spans="2:19" s="38" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -36164,14 +36162,14 @@
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
       <c r="F3" s="39"/>
-      <c r="N3" s="101" t="str">
+      <c r="N3" s="94" t="str">
         <f>IFERROR(CONCATENATE(VLOOKUP("remaining_credits",CNPJá___Conta[],2,0)," ₪"),"")</f>
         <v/>
       </c>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="101"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
       <c r="S3" s="69"/>
     </row>
     <row r="4" spans="2:19" s="38" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -36185,20 +36183,20 @@
       <c r="B6" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="102" t="s">
+      <c r="E6" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
     </row>
     <row r="7" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="48" t="str">
         <f>TEXT(COUNTA(cnpjaSource[]),"0")&amp;" registros"</f>
         <v>0 registros</v>
       </c>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
     </row>
     <row r="8" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="str">
@@ -36263,65 +36261,65 @@
       <c r="B14" s="45"/>
       <c r="C14" s="36"/>
       <c r="D14" s="15"/>
-      <c r="E14" s="102" t="s">
+      <c r="E14" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
     </row>
     <row r="15" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="45"/>
       <c r="C15" s="36"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="102"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
     </row>
     <row r="16" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="45"/>
       <c r="C16" s="36"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="96" t="s">
+      <c r="E16" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="100"/>
       <c r="I16" s="64"/>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="K16" s="96"/>
-      <c r="L16" s="96"/>
-      <c r="M16" s="96"/>
-      <c r="O16" s="96" t="s">
+      <c r="K16" s="100"/>
+      <c r="L16" s="100"/>
+      <c r="M16" s="100"/>
+      <c r="O16" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="P16" s="96"/>
-      <c r="Q16" s="96"/>
-      <c r="R16" s="96"/>
+      <c r="P16" s="100"/>
+      <c r="Q16" s="100"/>
+      <c r="R16" s="100"/>
     </row>
     <row r="17" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="45"/>
       <c r="C17" s="36"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="100"/>
       <c r="I17" s="64"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="100"/>
+      <c r="L17" s="100"/>
+      <c r="M17" s="100"/>
+      <c r="O17" s="100"/>
+      <c r="P17" s="100"/>
+      <c r="Q17" s="100"/>
+      <c r="R17" s="100"/>
     </row>
     <row r="18" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="45"/>
@@ -36383,42 +36381,42 @@
       <c r="B25" s="45"/>
       <c r="C25" s="36"/>
       <c r="D25" s="15"/>
-      <c r="E25" s="94" t="str">
+      <c r="E25" s="98" t="str">
         <f>CONCATENATE("?",IF(OpReceita[[#Totals],[Valor]]=0,"","company_max_age="&amp;OpReceita[[#Totals],[Valor]]),"&amp;",IF(OpSINTEGRA[[#Totals],[Valor]]=0,"","sintegra_max_age="&amp;OpSINTEGRA[[#Totals],[Valor]]),"&amp;",IF(OpSimples[[#Totals],[Valor]]=0,"","simples_max_age="&amp;OpSimples[[#Totals],[Valor]]))</f>
         <v>?&amp;&amp;</v>
       </c>
-      <c r="F25" s="94"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="94"/>
-      <c r="J25" s="94"/>
-      <c r="K25" s="94"/>
-      <c r="L25" s="94"/>
-      <c r="M25" s="94"/>
-      <c r="N25" s="94"/>
-      <c r="O25" s="94"/>
-      <c r="P25" s="94"/>
-      <c r="Q25" s="94"/>
-      <c r="R25" s="94"/>
-      <c r="S25" s="94"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="98"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="98"/>
+      <c r="M25" s="98"/>
+      <c r="N25" s="98"/>
+      <c r="O25" s="98"/>
+      <c r="P25" s="98"/>
+      <c r="Q25" s="98"/>
+      <c r="R25" s="98"/>
+      <c r="S25" s="98"/>
     </row>
     <row r="26" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="45"/>
       <c r="C26" s="36"/>
       <c r="D26" s="15"/>
-      <c r="E26" s="99" t="s">
+      <c r="E26" s="103" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="99"/>
-      <c r="J26" s="99"/>
-      <c r="K26" s="98" t="str">
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="103"/>
+      <c r="K26" s="102" t="str">
         <f>CONCATENATE(SUM(1,IF(OpSINTEGRA[[#Totals],[Valor]]=0,0,15),IF(OpSimples[[#Totals],[Valor]]=0,0,30))," ₪")</f>
         <v>1 ₪</v>
       </c>
-      <c r="L26" s="98"/>
+      <c r="L26" s="102"/>
     </row>
     <row r="27" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="45"/>
@@ -36447,59 +36445,59 @@
       <c r="B28" s="45"/>
       <c r="C28" s="36"/>
       <c r="D28" s="15"/>
-      <c r="E28" s="95" t="str">
+      <c r="E28" s="99" t="str">
         <f ca="1">IFERROR(INDEX(OpSINTEGRA[Descrição],MATCH(OpSINTEGRA[[#Totals],[Valor]],OpSINTEGRA[Valor],0)),"• [Erro] Selecione apenas uma opção em SINTEGRA.")</f>
         <v>• SINTEGRA retornará do Cache se disponível [ +0 ₪ ]</v>
       </c>
-      <c r="F28" s="95"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="95"/>
-      <c r="N28" s="95"/>
-      <c r="O28" s="95"/>
-      <c r="P28" s="95"/>
-      <c r="Q28" s="95"/>
-      <c r="R28" s="95"/>
-      <c r="S28" s="95"/>
-      <c r="T28" s="95"/>
-      <c r="U28" s="95"/>
-      <c r="V28" s="95"/>
-      <c r="W28" s="95"/>
-      <c r="X28" s="95"/>
-      <c r="Y28" s="95"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="99"/>
+      <c r="J28" s="99"/>
+      <c r="K28" s="99"/>
+      <c r="L28" s="99"/>
+      <c r="M28" s="99"/>
+      <c r="N28" s="99"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="99"/>
+      <c r="Q28" s="99"/>
+      <c r="R28" s="99"/>
+      <c r="S28" s="99"/>
+      <c r="T28" s="99"/>
+      <c r="U28" s="99"/>
+      <c r="V28" s="99"/>
+      <c r="W28" s="99"/>
+      <c r="X28" s="99"/>
+      <c r="Y28" s="99"/>
     </row>
     <row r="29" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="45"/>
       <c r="C29" s="36"/>
       <c r="D29" s="15"/>
-      <c r="E29" s="95" t="str">
+      <c r="E29" s="99" t="str">
         <f ca="1">IFERROR(INDEX(OpSimples[Descrição],MATCH(OpSimples[[#Totals],[Valor]],OpSimples[Valor],0)),"• [Erro] Selecione apenas uma opção em Simples Nacional.")</f>
         <v>• Simples Nacional retornará do Cache se disponível [ +0 ₪ ]</v>
       </c>
-      <c r="F29" s="95"/>
-      <c r="G29" s="95"/>
-      <c r="H29" s="95"/>
-      <c r="I29" s="95"/>
-      <c r="J29" s="95"/>
-      <c r="K29" s="95"/>
-      <c r="L29" s="95"/>
-      <c r="M29" s="95"/>
-      <c r="N29" s="95"/>
-      <c r="O29" s="95"/>
-      <c r="P29" s="95"/>
-      <c r="Q29" s="95"/>
-      <c r="R29" s="95"/>
-      <c r="S29" s="95"/>
-      <c r="T29" s="95"/>
-      <c r="U29" s="95"/>
-      <c r="V29" s="95"/>
-      <c r="W29" s="95"/>
-      <c r="X29" s="95"/>
-      <c r="Y29" s="95"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="99"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="99"/>
+      <c r="J29" s="99"/>
+      <c r="K29" s="99"/>
+      <c r="L29" s="99"/>
+      <c r="M29" s="99"/>
+      <c r="N29" s="99"/>
+      <c r="O29" s="99"/>
+      <c r="P29" s="99"/>
+      <c r="Q29" s="99"/>
+      <c r="R29" s="99"/>
+      <c r="S29" s="99"/>
+      <c r="T29" s="99"/>
+      <c r="U29" s="99"/>
+      <c r="V29" s="99"/>
+      <c r="W29" s="99"/>
+      <c r="X29" s="99"/>
+      <c r="Y29" s="99"/>
     </row>
     <row r="30" spans="2:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="45"/>
@@ -36513,13 +36511,13 @@
       <c r="B31" s="45"/>
       <c r="C31" s="36"/>
       <c r="D31" s="15"/>
-      <c r="E31" s="97" t="s">
+      <c r="E31" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="97"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="97"/>
-      <c r="I31" s="97"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
+      <c r="I31" s="101"/>
       <c r="J31" s="65"/>
       <c r="K31" s="65"/>
       <c r="L31" s="65"/>
@@ -36534,11 +36532,11 @@
       <c r="B32" s="45"/>
       <c r="C32" s="36"/>
       <c r="D32" s="15"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="101"/>
+      <c r="I32" s="101"/>
       <c r="J32" s="65"/>
       <c r="K32" s="65"/>
       <c r="L32" s="65"/>
@@ -36691,17 +36689,17 @@
     </row>
     <row r="49" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="45"/>
-      <c r="E49" s="102" t="s">
+      <c r="E49" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="102"/>
-      <c r="G49" s="102"/>
+      <c r="F49" s="95"/>
+      <c r="G49" s="95"/>
     </row>
     <row r="50" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="45"/>
-      <c r="E50" s="102"/>
-      <c r="F50" s="102"/>
-      <c r="G50" s="102"/>
+      <c r="E50" s="95"/>
+      <c r="F50" s="95"/>
+      <c r="G50" s="95"/>
     </row>
     <row r="51" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="45"/>
@@ -36849,13 +36847,13 @@
         <v>111</v>
       </c>
       <c r="F69" s="15"/>
-      <c r="N69" s="103" t="s">
+      <c r="N69" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="O69" s="103"/>
-      <c r="P69" s="103"/>
-      <c r="Q69" s="103"/>
-      <c r="R69" s="103"/>
+      <c r="O69" s="96"/>
+      <c r="P69" s="96"/>
+      <c r="Q69" s="96"/>
+      <c r="R69" s="96"/>
     </row>
     <row r="70" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="45"/>
@@ -36873,23 +36871,23 @@
     </row>
     <row r="72" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="45"/>
-      <c r="E72" s="93" t="s">
+      <c r="E72" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="F72" s="93"/>
-      <c r="G72" s="93"/>
-      <c r="H72" s="93"/>
-      <c r="I72" s="93"/>
-      <c r="J72" s="93"/>
-      <c r="K72" s="93"/>
-      <c r="L72" s="93"/>
-      <c r="M72" s="93"/>
-      <c r="N72" s="93"/>
-      <c r="O72" s="93"/>
-      <c r="P72" s="93"/>
-      <c r="Q72" s="93"/>
-      <c r="R72" s="93"/>
-      <c r="S72" s="93"/>
+      <c r="F72" s="97"/>
+      <c r="G72" s="97"/>
+      <c r="H72" s="97"/>
+      <c r="I72" s="97"/>
+      <c r="J72" s="97"/>
+      <c r="K72" s="97"/>
+      <c r="L72" s="97"/>
+      <c r="M72" s="97"/>
+      <c r="N72" s="97"/>
+      <c r="O72" s="97"/>
+      <c r="P72" s="97"/>
+      <c r="Q72" s="97"/>
+      <c r="R72" s="97"/>
+      <c r="S72" s="97"/>
     </row>
     <row r="73" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="45"/>
@@ -39707,12 +39705,6 @@
   </sheetData>
   <sheetProtection sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="16">
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="E49:G50"/>
-    <mergeCell ref="N69:R69"/>
-    <mergeCell ref="E14:I15"/>
-    <mergeCell ref="E6:G7"/>
     <mergeCell ref="E72:S72"/>
     <mergeCell ref="E25:S25"/>
     <mergeCell ref="E29:Y29"/>
@@ -39723,6 +39715,12 @@
     <mergeCell ref="E16:H17"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="E26:J26"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="E49:G50"/>
+    <mergeCell ref="N69:R69"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="E6:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N69" r:id="rId1" xr:uid="{764E0002-E7C3-41F0-B42B-D7E9AF39DCA8}"/>

</xml_diff>